<commit_message>
LA OK ! NB LIGNES OK !
</commit_message>
<xml_diff>
--- a/Base de données/insert into/LA.xlsx
+++ b/Base de données/insert into/LA.xlsx
@@ -16,93 +16,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="29">
-  <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>ENG</t>
-  </si>
-  <si>
-    <t>GER</t>
-  </si>
-  <si>
-    <t>FRE</t>
-  </si>
-  <si>
-    <t>SPA</t>
-  </si>
-  <si>
-    <t>ITA</t>
-  </si>
-  <si>
-    <t>RUS</t>
-  </si>
-  <si>
-    <t>CHI</t>
-  </si>
-  <si>
-    <t>UND</t>
-  </si>
-  <si>
-    <t>POR</t>
-  </si>
-  <si>
-    <t>POL</t>
-  </si>
-  <si>
-    <t>CZE</t>
-  </si>
-  <si>
-    <t>SLO</t>
-  </si>
-  <si>
-    <t>NOR</t>
-  </si>
-  <si>
-    <t>JPN</t>
-  </si>
-  <si>
-    <t>SWE</t>
-  </si>
-  <si>
-    <t>HRV</t>
-  </si>
-  <si>
-    <t>DUT</t>
-  </si>
-  <si>
-    <t>TUR</t>
-  </si>
-  <si>
-    <t>HUN</t>
-  </si>
-  <si>
-    <t>UKR</t>
-  </si>
-  <si>
-    <t>ROM</t>
-  </si>
-  <si>
-    <t>PERSIAN</t>
-  </si>
-  <si>
-    <t>GREC</t>
-  </si>
-  <si>
-    <t>FIN</t>
-  </si>
-  <si>
-    <t>DAN</t>
-  </si>
-  <si>
-    <t>ARABE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>INSERT INTO LA VALUES ('</t>
   </si>
   <si>
     <t>');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JPN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HRV </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DUT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TUR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UKR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERSIAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GREC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARABE </t>
   </si>
 </sst>
 </file>
@@ -443,303 +440,301 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A2:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C27"/>
+      <selection activeCell="A2" sqref="A2:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>